<commit_message>
Added chance and community cards loading
</commit_message>
<xml_diff>
--- a/MonopolySimulator/boardConfig.xlsx
+++ b/MonopolySimulator/boardConfig.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" sheetId="1" r:id="rId1"/>
+    <sheet name="Config" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
   <si>
     <t>Payout</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Connecticut Avenue</t>
   </si>
   <si>
-    <t>In Jail</t>
-  </si>
-  <si>
-    <t>Just Visiting Jail</t>
-  </si>
-  <si>
     <t>Community</t>
   </si>
   <si>
@@ -166,6 +160,45 @@
   </si>
   <si>
     <t>Property</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>NextUtility</t>
+  </si>
+  <si>
+    <t>Railroad</t>
+  </si>
+  <si>
+    <t>NextRailroad</t>
+  </si>
+  <si>
+    <t>JailCard</t>
+  </si>
+  <si>
+    <t>Goto1</t>
+  </si>
+  <si>
+    <t>Goto26</t>
+  </si>
+  <si>
+    <t>Goto13</t>
+  </si>
+  <si>
+    <t>Move-3</t>
+  </si>
+  <si>
+    <t>Goto6</t>
+  </si>
+  <si>
+    <t>Goto41</t>
+  </si>
+  <si>
+    <t>GotoJail</t>
+  </si>
+  <si>
+    <t>Ignore</t>
   </si>
 </sst>
 </file>
@@ -285,7 +318,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -569,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,9 +666,11 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -600,8 +686,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -609,14 +701,20 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>200</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -624,14 +722,20 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>60</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -639,14 +743,20 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -654,14 +764,20 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>60</v>
       </c>
       <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -669,14 +785,20 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>-200</v>
       </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -684,14 +806,20 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>200</v>
       </c>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -699,14 +827,20 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -720,8 +854,14 @@
         <v>0</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -729,14 +869,20 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>100</v>
       </c>
       <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -744,352 +890,400 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11">
         <v>120</v>
       </c>
       <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14">
-        <v>140</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15">
-        <v>150</v>
-      </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17">
-        <v>160</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="G17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D18">
-        <v>200</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="G18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D19">
-        <v>180</v>
-      </c>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22">
-        <v>200</v>
-      </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D24">
-        <v>220</v>
-      </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D26">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27">
-        <v>240</v>
-      </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28">
-        <v>200</v>
-      </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D29">
         <v>260</v>
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30">
-        <v>260</v>
-      </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D31">
-        <v>150</v>
-      </c>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D32">
-        <v>280</v>
-      </c>
-      <c r="E32" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D34">
         <v>300</v>
@@ -1101,58 +1295,58 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D35">
-        <v>300</v>
-      </c>
-      <c r="E35" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>320</v>
+      </c>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D37">
-        <v>320</v>
-      </c>
-      <c r="E37" s="10"/>
+        <v>200</v>
+      </c>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="D38">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="E38" s="1"/>
     </row>
@@ -1161,67 +1355,60 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>350</v>
+      </c>
+      <c r="E39" s="11"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D40">
-        <v>350</v>
-      </c>
-      <c r="E40" s="11"/>
+        <v>-100</v>
+      </c>
+      <c r="E40" s="1"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
       </c>
       <c r="D41">
-        <v>-100</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42">
-        <v>400</v>
-      </c>
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>47</v>
+      <c r="A42" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G2:H17">
+    <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="Ignore">
+      <formula>ISERROR(SEARCH("Ignore",G2))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Ignore">
+      <formula>NOT(ISERROR(SEARCH("Ignore",G2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added all basic mechanics,will add tomorrow double dice,triple dice,community and chance cards
</commit_message>
<xml_diff>
--- a/MonopolySimulator/boardConfig.xlsx
+++ b/MonopolySimulator/boardConfig.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t>Payout</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Broadwalk</t>
-  </si>
-  <si>
-    <t>GoJail</t>
   </si>
   <si>
     <t>Tax</t>
@@ -655,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,10 +705,10 @@
       </c>
       <c r="E2" s="1"/>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -722,17 +719,17 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>60</v>
       </c>
       <c r="E3" s="2"/>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,10 +747,10 @@
       </c>
       <c r="E4" s="1"/>
       <c r="G4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -764,17 +761,17 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>60</v>
       </c>
       <c r="E5" s="4"/>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -785,17 +782,17 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>-200</v>
       </c>
       <c r="E6" s="1"/>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,17 +803,17 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>200</v>
       </c>
       <c r="E7" s="1"/>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -827,17 +824,17 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8">
         <v>100</v>
       </c>
       <c r="E8" s="5"/>
       <c r="G8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -855,10 +852,10 @@
       </c>
       <c r="E9" s="1"/>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -869,17 +866,17 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>100</v>
       </c>
       <c r="E10" s="5"/>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -890,17 +887,17 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11">
         <v>120</v>
       </c>
       <c r="E11" s="5"/>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -918,10 +915,10 @@
       </c>
       <c r="E12" s="1"/>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -932,17 +929,17 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>140</v>
       </c>
       <c r="E13" s="6"/>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -953,17 +950,17 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>150</v>
       </c>
       <c r="E14" s="1"/>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,17 +971,17 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>140</v>
       </c>
       <c r="E15" s="6"/>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -995,17 +992,17 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>160</v>
       </c>
       <c r="E16" s="6"/>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,17 +1013,17 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17">
         <v>200</v>
       </c>
       <c r="E17" s="1"/>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1037,17 +1034,17 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18">
         <v>180</v>
       </c>
       <c r="E18" s="7"/>
       <c r="G18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1073,7 +1070,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20">
         <v>180</v>
@@ -1088,7 +1085,7 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21">
         <v>200</v>
@@ -1103,7 +1100,7 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1118,7 +1115,7 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>220</v>
@@ -1148,7 +1145,7 @@
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25">
         <v>220</v>
@@ -1163,7 +1160,7 @@
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26">
         <v>240</v>
@@ -1178,7 +1175,7 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>200</v>
@@ -1193,7 +1190,7 @@
         <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>260</v>
@@ -1208,7 +1205,7 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29">
         <v>260</v>
@@ -1223,7 +1220,7 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30">
         <v>150</v>
@@ -1238,7 +1235,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31">
         <v>280</v>
@@ -1253,7 +1250,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1268,7 +1265,7 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33">
         <v>300</v>
@@ -1283,7 +1280,7 @@
         <v>37</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D34">
         <v>300</v>
@@ -1313,7 +1310,7 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36">
         <v>320</v>
@@ -1328,7 +1325,7 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37">
         <v>200</v>
@@ -1358,7 +1355,7 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39">
         <v>350</v>
@@ -1373,7 +1370,7 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D40">
         <v>-100</v>
@@ -1388,7 +1385,7 @@
         <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D41">
         <v>400</v>
@@ -1397,7 +1394,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results window and processing percentage
</commit_message>
<xml_diff>
--- a/MonopolySimulator/boardConfig.xlsx
+++ b/MonopolySimulator/boardConfig.xlsx
@@ -315,17 +315,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -362,7 +352,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -652,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,14 +1388,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:H17">
-    <cfRule type="notContainsText" dxfId="2" priority="2" operator="notContains" text="Ignore">
-      <formula>ISERROR(SEARCH("Ignore",G2))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Ignore">
-      <formula>NOT(ISERROR(SEARCH("Ignore",G2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>